<commit_message>
lagt til kommuner med egen farge på søyler
</commit_message>
<xml_diff>
--- a/data/el-forbruk.xlsx
+++ b/data/el-forbruk.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sintefrune/Code/elektrisk_energi_grenland/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE8EB8A-C5AA-7D46-B394-8B0E51CE8810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE8744D-7EC7-014C-93BE-F9DCA61CD5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="760" windowWidth="29780" windowHeight="20800" xr2:uid="{441BB446-576D-4888-8037-B5A9B0E2A856}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="29780" windowHeight="20800" activeTab="1" xr2:uid="{441BB446-576D-4888-8037-B5A9B0E2A856}"/>
   </bookViews>
   <sheets>
     <sheet name="liste-over-forbrukere" sheetId="2" r:id="rId1"/>
+    <sheet name="forbrukere-og-kommuner" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="55">
   <si>
     <t>Bedrift</t>
   </si>
@@ -169,13 +170,43 @@
   </si>
   <si>
     <t>https://e24.no/energi-og-klima/i/xg4O9X/hydro-om-batteri-investering-finnes-ikke-baerekraftige-alternativer-til-vianode-i-europa</t>
+  </si>
+  <si>
+    <t>farge</t>
+  </si>
+  <si>
+    <t>Oslo kommune totalt</t>
+  </si>
+  <si>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>https://www.ssb.no/statbank/table/10314/tableViewLayout1/</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>Trondheim kommune totalt</t>
+  </si>
+  <si>
+    <t>Trondheim</t>
+  </si>
+  <si>
+    <t>skyblue</t>
+  </si>
+  <si>
+    <t>Skien kommune totalt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +237,34 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9203FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9203FF"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -262,6 +321,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
@@ -579,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA66D0AE-0F44-46B7-90B8-EF3648A5FB53}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -944,7 +1019,523 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB910CCB-4D0E-204E-B8D9-85272DFA7143}">
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="12">
+        <v>8419000</v>
+      </c>
+      <c r="C2" s="13">
+        <v>2022</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6">
+        <v>7533600</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3942000</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="12">
+        <v>2784000</v>
+      </c>
+      <c r="C5" s="13">
+        <v>2022</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="6">
+        <v>998640</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>925538</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2020</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>682556</v>
+      </c>
+      <c r="C8" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="12">
+        <v>646900</v>
+      </c>
+      <c r="C9" s="11">
+        <v>2022</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>550282</v>
+      </c>
+      <c r="C10" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2">
+        <v>244312</v>
+      </c>
+      <c r="C11" s="10">
+        <v>2021</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="2">
+        <v>198259</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2020</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>156495</v>
+      </c>
+      <c r="C13" s="10">
+        <v>2021</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2">
+        <v>37328</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2020</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2">
+        <v>11111</v>
+      </c>
+      <c r="C15" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="2">
+        <v>11110</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="2">
+        <v>6664</v>
+      </c>
+      <c r="C17" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4270</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3">
+        <v>910</v>
+      </c>
+      <c r="C19" s="10">
+        <v>2022</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3">
+        <v>189</v>
+      </c>
+      <c r="C20" s="10">
+        <v>2021</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{CE0DBE3E-8432-CA4F-A795-C67E7DE265BB}"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://www.ta.no/kan-bli-norges-storste-stromforbruker-google-har-sokt-om-860-megawatt-over-fire-ganger-sa-mye-strom-som-all-industri-pa-heroya/s/5-50-1736371" xr:uid="{D62A4EE3-02BD-3F4F-886F-802E8E96CD12}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://montelnews.com/no/news/1448850/statnett-gir-yara-nettkobling-til-hegra-prosjektet-4-twh" xr:uid="{D5BE1B5F-1CF6-7E40-A753-DAA9DCBB3728}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{ADB46F58-2B5F-E549-A2FF-9D80022D4845}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{895DB7B9-5956-B241-A7EC-D541EFF67819}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{E24C88DB-8F1C-6046-B597-3E82ABD002E0}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{7A00724B-F382-A444-B867-00867BFAB2AF}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{F00B58CF-D434-4549-A464-2151F55A4632}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{5C699539-518C-CC4E-B3CB-F5D30DFEFECC}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{7B5A88BB-8CA1-6A4D-AF1A-8EED435513E1}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{B35B2639-7973-E84D-956B-00910AE3BC01}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{FD418FE8-BFED-3A49-9191-950977D702E2}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{36256220-D414-0040-8EAC-6D079812B659}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{9DE50A56-E41B-614A-B0B1-7CC2074839D6}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{898A35BB-C815-3D40-AD3C-273CB6A5B657}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{FF27080B-8E7E-1740-AE36-E129A0ABF58D}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{DF630C7E-CF9E-1C43-A0AC-CECDE4A3E276}"/>
+    <hyperlink ref="F20" r:id="rId18" xr:uid="{94C697DB-71AB-6A42-85F2-A823A3641303}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectLeader>
+    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
+    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectOwner>
+    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
+    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
+    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
+    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
+    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteDocumentAuthor>
+    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <ArchiveRecNo xmlns="3ffbde1b-7654-42c0-8074-5badcf74c2df" xsi:nil="true"/>
+    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </CorpSiteProjectQA>
+    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
+    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Generic document" ma:contentTypeID="0x01010031B82B69D2361148B4D8F7EC156802130800F3E3B1C9150D2344B1E06DE395297CC7" ma:contentTypeVersion="42" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="54637571ad3c887385810f4277aa4707">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8bbd4995-53b7-43e2-b62f-10947586ac31" xmlns:ns3="3ffbde1b-7654-42c0-8074-5badcf74c2df" xmlns:ns4="65bac99c-89d4-4af4-bc61-b1a523cd4bb3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c4cc8d1dd8650c3a19a4728e75cfb4b8" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
@@ -1467,96 +2058,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <CorpSiteZipContact xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectLeader xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectLeader>
-    <CorpSiteSubTitle xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteTags xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteISBN xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowFeedback xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteAccess xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Kun navngitte medlemmer</CorpSiteAccess>
-    <CorpSiteRecipientPerson xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectName xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocInstitute xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteInstitutePhone xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectOwner xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectOwner>
-    <CorpDocPageClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocPageClassificationNbNo>
-    <CorpDocClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocClassificationEnUs>
-    <CorpDocClassificationNbNo xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpDocClassificationNbNo>
-    <CorpWorkflowStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteClassification xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Åpen</CorpSiteClassification>
-    <CorpSiteInstituteEmail xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteCoAuthors xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocumentAuthor xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteDocumentAuthor>
-    <CorpSiteInstituteEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <ArchiveRecNo xmlns="3ffbde1b-7654-42c0-8074-5badcf74c2df" xsi:nil="true"/>
-    <CorpSiteRecipientCompany xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteDocLanguage xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocVersion xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpWorkflowApproval xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <ArchiveStatus xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteProjectQA xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </CorpSiteProjectQA>
-    <CorpSiteZipAddress xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteVATNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteReportNumber xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpSiteOurRef xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31" xsi:nil="true"/>
-    <CorpDocPageClassificationEnUs xmlns="8bbd4995-53b7-43e2-b62f-10947586ac31">Unrestricted</CorpDocPageClassificationEnUs>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{152E9083-380C-43BC-89A9-8FEA692C580A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E1507F3-CB8F-4C78-85C7-A280106EFC39}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
-    <ds:schemaRef ds:uri="3ffbde1b-7654-42c0-8074-5badcf74c2df"/>
-    <ds:schemaRef ds:uri="65bac99c-89d4-4af4-bc61-b1a523cd4bb3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1580,9 +2085,21 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E1507F3-CB8F-4C78-85C7-A280106EFC39}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{152E9083-380C-43BC-89A9-8FEA692C580A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8bbd4995-53b7-43e2-b62f-10947586ac31"/>
+    <ds:schemaRef ds:uri="3ffbde1b-7654-42c0-8074-5badcf74c2df"/>
+    <ds:schemaRef ds:uri="65bac99c-89d4-4af4-bc61-b1a523cd4bb3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>